<commit_message>
First commit for 4th march 2017
</commit_message>
<xml_diff>
--- a/Neha_Pant.xlsx
+++ b/Neha_Pant.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="177">
   <si>
     <t>S.No</t>
   </si>
@@ -472,6 +472,90 @@
   </si>
   <si>
     <t>Java configuration for hibernate in backend</t>
+  </si>
+  <si>
+    <t>4th Mar,2017</t>
+  </si>
+  <si>
+    <t>MVC Concept</t>
+  </si>
+  <si>
+    <t>View for requestparam and pathvariable</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=IXg52Lg58m4</t>
+  </si>
+  <si>
+    <t>Creation of landing page and loading static resources</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=OuSElmnstN8</t>
+  </si>
+  <si>
+    <t>Creation of master page</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=qACqz8bMqSM&amp;t=1s</t>
+  </si>
+  <si>
+    <t>Creation of active menu</t>
+  </si>
+  <si>
+    <t>70 minutes</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=zjiFBiNxdMI</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=F2L24Cy4zkQ</t>
+  </si>
+  <si>
+    <t>Adding dependencies</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=STi8nP7yArs&amp;t=38s</t>
+  </si>
+  <si>
+    <t>Linking backend project with UI</t>
+  </si>
+  <si>
+    <t>Side bar creation</t>
+  </si>
+  <si>
+    <t>Adding dependency inject @Autowired</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=t15lMwO7Q28</t>
+  </si>
+  <si>
+    <t>Adding dynamic url for products</t>
+  </si>
+  <si>
+    <t>Creating DTO and DAO classes fro Products</t>
+  </si>
+  <si>
+    <t>Creating DTO and DAO classes fro Category</t>
+  </si>
+  <si>
+    <t>Design Products.jsp</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=CV0g70poh_g&amp;t=253s</t>
+  </si>
+  <si>
+    <t>Configuring hibernate to work with h2</t>
+  </si>
+  <si>
+    <t>Making project functional till view all products</t>
+  </si>
+  <si>
+    <t>Images_Error</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=CuygFw_H9hk</t>
+  </si>
+  <si>
+    <t>Write test cases to work with ProductDAO</t>
   </si>
 </sst>
 </file>
@@ -961,7 +1045,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -969,10 +1053,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2263,6 +2347,469 @@
       </c>
       <c r="F51" s="1" t="s">
         <v>118</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="28.8">
+      <c r="A52" s="1">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="28.8">
+      <c r="A53" s="1">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="28.8">
+      <c r="A54" s="1">
+        <v>53</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="28.8">
+      <c r="A55" s="1">
+        <v>54</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="28.8">
+      <c r="A56" s="1">
+        <v>55</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="28.8">
+      <c r="A57" s="1">
+        <v>56</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="28.8">
+      <c r="A58" s="1">
+        <v>57</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="28.8">
+      <c r="A59" s="1">
+        <v>58</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="28.8">
+      <c r="A60" s="1">
+        <v>59</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="28.8">
+      <c r="A61" s="1">
+        <v>60</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="28.8">
+      <c r="A62" s="1">
+        <v>61</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="28.8">
+      <c r="A63" s="1">
+        <v>62</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="28.8">
+      <c r="A64" s="1">
+        <v>63</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="28.8">
+      <c r="A65" s="1">
+        <v>64</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="28.8">
+      <c r="A66" s="1">
+        <v>65</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="28.8">
+      <c r="A67" s="1">
+        <v>66</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="28.8">
+      <c r="A68" s="1">
+        <v>67</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="28.8">
+      <c r="A69" s="1">
+        <v>68</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" s="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" s="1">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2288,8 +2835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A7" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Third commit for 4th march 2017
</commit_message>
<xml_diff>
--- a/Neha_Pant.xlsx
+++ b/Neha_Pant.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="180">
   <si>
     <t>S.No</t>
   </si>
@@ -556,6 +556,15 @@
   </si>
   <si>
     <t>Write test cases to work with ProductDAO</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=S9wKr2nuHHw&amp;t=25s</t>
+  </si>
+  <si>
+    <t>Images were not displayed after doing all the static resource loading</t>
+  </si>
+  <si>
+    <t>Ctrl+F5 in the browser , this clears the cache</t>
   </si>
 </sst>
 </file>
@@ -1045,7 +1054,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1055,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView tabSelected="1" topLeftCell="D59" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H70" sqref="H70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2801,10 +2810,46 @@
       <c r="C69" s="1" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="70" spans="1:8">
+      <c r="D69" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="28.8">
       <c r="A70" s="1">
         <v>69</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2974,8 +3019,19 @@
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="C10"/>
+    <row r="10" spans="1:5" ht="28.8">
+      <c r="A10" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="C11"/>

</xml_diff>

<commit_message>
First commit for 5th march 2017
</commit_message>
<xml_diff>
--- a/Neha_Pant.xlsx
+++ b/Neha_Pant.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="189">
   <si>
     <t>S.No</t>
   </si>
@@ -565,6 +565,33 @@
   </si>
   <si>
     <t>Ctrl+F5 in the browser , this clears the cache</t>
+  </si>
+  <si>
+    <t>5th Mar,2017</t>
+  </si>
+  <si>
+    <t>Hibernate form validation session</t>
+  </si>
+  <si>
+    <t>http://websystique.com/springmvc/spring-4-mvc-form-validation-with-hibernate-jsr-validator-resource-handling-using-annotations/</t>
+  </si>
+  <si>
+    <t>CRUD using hibernate</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=rdYQOqxq9F0</t>
+  </si>
+  <si>
+    <t>Spring Forms</t>
+  </si>
+  <si>
+    <t>CRUD with spring forms-add</t>
+  </si>
+  <si>
+    <t>CRUD with spring forms-view with datatable</t>
+  </si>
+  <si>
+    <t>Hibernate form validation-dependency setup</t>
   </si>
 </sst>
 </file>
@@ -1054,7 +1081,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1062,10 +1089,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H71"/>
+  <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D59" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H70" sqref="H70"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2852,9 +2879,200 @@
         <v>19</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" ht="28.8">
       <c r="A71" s="1">
         <v>70</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="28.8">
+      <c r="A72" s="1">
+        <v>71</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D72" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="28.8">
+      <c r="A73" s="1">
+        <v>72</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="28.8">
+      <c r="A74" s="1">
+        <v>73</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="28.8">
+      <c r="A75" s="1">
+        <v>74</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="28.8">
+      <c r="A76" s="1">
+        <v>75</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="28.8">
+      <c r="A77" s="1">
+        <v>76</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="28.8">
+      <c r="A78" s="1">
+        <v>77</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="28.8">
+      <c r="A79" s="1">
+        <v>78</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="28.8">
+      <c r="A80" s="1">
+        <v>79</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="28.8">
+      <c r="A81" s="1">
+        <v>80</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2870,9 +3088,10 @@
     <hyperlink ref="D22" r:id="rId9" display="https://www.youtube.com/watch?v=9fVQ_mvzV48 "/>
     <hyperlink ref="D43" r:id="rId10"/>
     <hyperlink ref="D47" r:id="rId11" tooltip="https://www.youtube.com/watch?v=oPE6UO9yoK4" display="https://www.youtube.com/watch?v=oPE6UO9yoK4"/>
+    <hyperlink ref="D72" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
First commit for 6th march 2017
</commit_message>
<xml_diff>
--- a/Neha_Pant.xlsx
+++ b/Neha_Pant.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="218">
   <si>
     <t>S.No</t>
   </si>
@@ -593,12 +593,104 @@
   <si>
     <t>Hibernate form validation-dependency setup</t>
   </si>
+  <si>
+    <t>6th Mar,2017</t>
+  </si>
+  <si>
+    <t>Hibernate validator correction</t>
+  </si>
+  <si>
+    <t>UnsatisfiedDependencyException_Error</t>
+  </si>
+  <si>
+    <t>UnsatisfiedDependencyException raised by code after adding validator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code:&lt;dependency&gt;
+    &lt;groupId&gt;org.jboss.logging&lt;/groupId&gt;
+    &lt;artifactId&gt;jboss-logging&lt;/artifactId&gt;
+    &lt;version&gt;3.3.0.Final&lt;/version&gt;
+&lt;/dependency&gt;
+</t>
+  </si>
+  <si>
+    <t>http://stackoverflow.com/questions/31547015/hibernate-5-java-lang-nosuchmethoderror-org-jboss-logging-logger-debugf</t>
+  </si>
+  <si>
+    <t>ValidModelAttribute_Error</t>
+  </si>
+  <si>
+    <t>Validator_Error</t>
+  </si>
+  <si>
+    <t>@ModelAttribute("product") @Valid Product product</t>
+  </si>
+  <si>
+    <t>valid and modelattribute were not working</t>
+  </si>
+  <si>
+    <t>Validator was working but the errors were not displayed in the form</t>
+  </si>
+  <si>
+    <t>Add the following code inside the doAction() of ProductController class : if(result.hasErrors()) {    ModelAndView model1 =new ModelAndView("page");    model1.addObject("title","Product Management");    model1.addObject("title","Product Management");    model1.addObject("userClickProductCRUD","true");             return model1;}</t>
+  </si>
+  <si>
+    <t>UnsatisfiedDependencyException_Error,ValiModelAttribute_Error,Validator_Error</t>
+  </si>
+  <si>
+    <t>270 minutes</t>
+  </si>
+  <si>
+    <t>Multipart Image upload</t>
+  </si>
+  <si>
+    <t>Multipart Image upload-Dependencies addition</t>
+  </si>
+  <si>
+    <t>https://mvnrepository.com      </t>
+  </si>
+  <si>
+    <t>MultipartUpload_Error</t>
+  </si>
+  <si>
+    <t>Image was not uploading</t>
+  </si>
+  <si>
+    <t>annotation from productImage has to be removed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://javabeat.net/spring-multipart-file-upload/ http://websystique.com/springmvc/spring-mvc-4-file-upload-example-using-commons-fileupload/ </t>
+  </si>
+  <si>
+    <t>Understanding webflow</t>
+  </si>
+  <si>
+    <t>http://www.jcombat.com/spring/create-your-first-spring-web-flow-based-web-application  http://www.springbyexample.org/examples/simple-spring-web-flow-webapp-http://www.springbyexample.org/examples/simple-spring-web-flow-webapp-spring-config.html      spring-config.html      </t>
+  </si>
+  <si>
+    <t>Creation of registration page</t>
+  </si>
+  <si>
+    <t>User model creation</t>
+  </si>
+  <si>
+    <t>User DAO creation</t>
+  </si>
+  <si>
+    <t>User DAOIMPL</t>
+  </si>
+  <si>
+    <t>Updation of navbar to add admin section</t>
+  </si>
+  <si>
+    <t>5 minutes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -638,6 +730,12 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -714,7 +812,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -752,9 +850,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -778,6 +873,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1089,10 +1195,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H81"/>
+  <dimension ref="A1:H87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1120,7 +1226,7 @@
       <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -1146,10 +1252,10 @@
       <c r="D2" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="18" t="s">
+      <c r="E2" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="17" t="s">
         <v>32</v>
       </c>
       <c r="G2" s="13" t="s">
@@ -1172,7 +1278,7 @@
       <c r="D3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -1198,7 +1304,7 @@
       <c r="D4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F4" s="8" t="s">
@@ -1250,7 +1356,7 @@
       <c r="D6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="4" t="s">
         <v>31</v>
       </c>
       <c r="F6" s="8" t="s">
@@ -1276,7 +1382,7 @@
       <c r="D7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F7" s="8" t="s">
@@ -1348,7 +1454,7 @@
       <c r="B10" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="19" t="s">
         <v>61</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -1663,7 +1769,7 @@
       <c r="C22" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D22" s="21" t="s">
+      <c r="D22" s="20" t="s">
         <v>88</v>
       </c>
       <c r="E22" s="1" t="s">
@@ -2185,7 +2291,7 @@
       <c r="C43" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D43" s="21" t="s">
+      <c r="D43" s="20" t="s">
         <v>133</v>
       </c>
       <c r="E43" s="1" t="s">
@@ -2223,7 +2329,7 @@
       <c r="G44" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H44" s="23" t="s">
+      <c r="H44" s="22" t="s">
         <v>125</v>
       </c>
     </row>
@@ -2249,7 +2355,7 @@
       <c r="G45" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2301,7 +2407,7 @@
       <c r="G47" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H47" s="23" t="s">
+      <c r="H47" s="22" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3040,15 +3146,51 @@
         <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" ht="28.8">
+        <v>189</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="57.6">
       <c r="A78" s="1">
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>180</v>
+        <v>189</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="28.8">
@@ -3056,23 +3198,233 @@
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" ht="28.8">
+        <v>189</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E79" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="43.2">
       <c r="A80" s="1">
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" ht="28.8">
+        <v>189</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H80" s="27" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="72">
       <c r="A81" s="1">
         <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>180</v>
+        <v>189</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E81" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="28.8">
+      <c r="A82" s="1">
+        <v>81</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E82" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="28.8">
+      <c r="A83" s="1">
+        <v>82</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E83" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="28.8">
+      <c r="A84" s="1">
+        <v>83</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E84" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="28.8">
+      <c r="A85" s="1">
+        <v>84</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E85" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="28.8">
+      <c r="A86" s="1">
+        <v>85</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E86" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="28.8">
+      <c r="A87" s="1">
+        <v>86</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E87" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -3089,18 +3441,20 @@
     <hyperlink ref="D43" r:id="rId10"/>
     <hyperlink ref="D47" r:id="rId11" tooltip="https://www.youtube.com/watch?v=oPE6UO9yoK4" display="https://www.youtube.com/watch?v=oPE6UO9yoK4"/>
     <hyperlink ref="D72" r:id="rId12"/>
+    <hyperlink ref="E79" r:id="rId13" tooltip="https://mvnrepository.com/" display="https://mvnrepository.com/"/>
+    <hyperlink ref="E81"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="A9" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3113,13 +3467,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="11" t="s">
@@ -3130,7 +3484,7 @@
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>28</v>
       </c>
       <c r="C2" s="10" t="s">
@@ -3144,7 +3498,7 @@
       <c r="A3" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>81</v>
       </c>
       <c r="C3" s="10" t="s">
@@ -3158,13 +3512,13 @@
       <c r="A4" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>97</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="20" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3186,7 +3540,7 @@
       <c r="A6" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="21" t="s">
         <v>107</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -3197,13 +3551,13 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="23.4" customHeight="1">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="23" t="s">
         <v>126</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -3211,7 +3565,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="40.799999999999997" customHeight="1">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="22" t="s">
         <v>128</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -3225,13 +3579,13 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="36.75" customHeight="1">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="22" t="s">
         <v>140</v>
       </c>
       <c r="B9" t="s">
         <v>141</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="26" t="s">
         <v>142</v>
       </c>
       <c r="D9" s="12" t="s">
@@ -3245,44 +3599,94 @@
       <c r="B10" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="26" t="s">
         <v>179</v>
       </c>
-      <c r="D10" s="27" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="C11"/>
+      <c r="D10" s="26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="86.4">
+      <c r="A11" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="C12" s="26"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="C13"/>
-      <c r="D13" s="26"/>
+      <c r="A12" s="27" t="s">
+        <v>195</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="79.2">
+      <c r="A13" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>200</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="C14"/>
-      <c r="E14" s="26"/>
+      <c r="A14" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>208</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="25"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="C15"/>
-      <c r="D15" s="26"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="25"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="C16"/>
+      <c r="C16" s="29"/>
     </row>
     <row r="17" spans="3:3">
-      <c r="C17"/>
+      <c r="C17" s="29"/>
+    </row>
+    <row r="18" spans="3:3">
+      <c r="C18" s="29"/>
+    </row>
+    <row r="19" spans="3:3">
+      <c r="C19" s="29"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="https://gist.github.com/adamjohnson/5682757"/>
     <hyperlink ref="D9" r:id="rId2" tooltip="https://www.youtube.com/watch?v=oPE6UO9yoK4" display="https://www.youtube.com/watch?v=oPE6UO9yoK4"/>
+    <hyperlink ref="D11" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
First commit for 7th march 2017
</commit_message>
<xml_diff>
--- a/Neha_Pant.xlsx
+++ b/Neha_Pant.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="231">
   <si>
     <t>S.No</t>
   </si>
@@ -684,6 +684,45 @@
   </si>
   <si>
     <t>5 minutes</t>
+  </si>
+  <si>
+    <t>7th Mar,2017</t>
+  </si>
+  <si>
+    <t>Modification of User entity class</t>
+  </si>
+  <si>
+    <t>Modification of UserDAOImpl class</t>
+  </si>
+  <si>
+    <t>Test cases for UserDAOImpl</t>
+  </si>
+  <si>
+    <t>Updation of test cases for ProductDAOImpl</t>
+  </si>
+  <si>
+    <t>Run the register page to register as supplier and customer</t>
+  </si>
+  <si>
+    <t>Create front end user controller</t>
+  </si>
+  <si>
+    <t>http://www.jcombat.com/spring/create-your-first-spring-web-flow-based-web-application</t>
+  </si>
+  <si>
+    <t>Configuration of webflow</t>
+  </si>
+  <si>
+    <t>Designed billing,welcome,navbar,preRegister pages</t>
+  </si>
+  <si>
+    <t>Creation of memberShipFlow.xml</t>
+  </si>
+  <si>
+    <t>Creation of address model</t>
+  </si>
+  <si>
+    <t>Creation of registerModel</t>
   </si>
 </sst>
 </file>
@@ -1187,7 +1226,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1195,10 +1234,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H87"/>
+  <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3427,6 +3466,298 @@
         <v>19</v>
       </c>
     </row>
+    <row r="88" spans="1:8" ht="28.8">
+      <c r="A88" s="1">
+        <v>87</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="28.8">
+      <c r="A89" s="1">
+        <v>88</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="28.8">
+      <c r="A90" s="1">
+        <v>89</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="28.8">
+      <c r="A91" s="1">
+        <v>90</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="28.8">
+      <c r="A92" s="1">
+        <v>91</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="28.8">
+      <c r="A93" s="1">
+        <v>92</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="28.8">
+      <c r="A94" s="1">
+        <v>93</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="43.2">
+      <c r="A95" s="1">
+        <v>94</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="28.8">
+      <c r="A96" s="1">
+        <v>95</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="28.8">
+      <c r="A97" s="1">
+        <v>96</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="28.8">
+      <c r="A98" s="1">
+        <v>97</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8">
+      <c r="A99" s="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8">
+      <c r="A100" s="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8">
+      <c r="A101" s="1">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1" display="https://www.youtube.com/watch?v=wx1UU7hhvbA"/>
@@ -3442,7 +3773,7 @@
     <hyperlink ref="D47" r:id="rId11" tooltip="https://www.youtube.com/watch?v=oPE6UO9yoK4" display="https://www.youtube.com/watch?v=oPE6UO9yoK4"/>
     <hyperlink ref="D72" r:id="rId12"/>
     <hyperlink ref="E79" r:id="rId13" tooltip="https://mvnrepository.com/" display="https://mvnrepository.com/"/>
-    <hyperlink ref="E81"/>
+    <hyperlink ref="E81" display="http://www.jcombat.com/spring/create-your-first-spring-web-flow-based-web-application  http://www.springbyexample.org/examples/simple-spring-web-flow-webapp-http://www.springbyexample.org/examples/simple-spring-web-flow-webapp-spring-config.html      spri"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId14"/>

</xml_diff>

<commit_message>
Committed on 08th March 2017
</commit_message>
<xml_diff>
--- a/Neha_Pant.xlsx
+++ b/Neha_Pant.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="234">
   <si>
     <t>S.No</t>
   </si>
@@ -723,6 +723,15 @@
   </si>
   <si>
     <t>Creation of registerModel</t>
+  </si>
+  <si>
+    <t>Creation of RegisterHandler</t>
+  </si>
+  <si>
+    <t>8th Mar,2017</t>
+  </si>
+  <si>
+    <t>Creation of Excepiton.jsp page</t>
   </si>
 </sst>
 </file>
@@ -1226,7 +1235,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1237,7 +1246,7 @@
   <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B99" sqref="B99"/>
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3742,15 +3751,66 @@
       <c r="E98" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="99" spans="1:8">
+      <c r="F98" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="28.8">
       <c r="A99" s="1">
         <v>98</v>
       </c>
-    </row>
-    <row r="100" spans="1:8">
+      <c r="B99" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="28.8">
       <c r="A100" s="1">
         <v>99</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H100" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="101" spans="1:8">

</xml_diff>

<commit_message>
First commit for 8th march 2017
</commit_message>
<xml_diff>
--- a/Neha_Pant.xlsx
+++ b/Neha_Pant.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="237">
   <si>
     <t>S.No</t>
   </si>
@@ -732,6 +732,15 @@
   </si>
   <si>
     <t>Creation of Excepiton.jsp page</t>
+  </si>
+  <si>
+    <t>Testing webflow till registration page</t>
+  </si>
+  <si>
+    <t>Created Address DAO,DTO and DAOIMPL and tested</t>
+  </si>
+  <si>
+    <t>Configured billing page with webflow</t>
   </si>
 </sst>
 </file>
@@ -1235,7 +1244,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1243,10 +1252,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H101"/>
+  <dimension ref="A1:H103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100"/>
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3813,9 +3822,82 @@
         <v>19</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" ht="28.8">
       <c r="A101" s="1">
         <v>100</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H101" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="28.8">
+      <c r="A102" s="1">
+        <v>101</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H102" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="28.8">
+      <c r="A103" s="1">
+        <v>102</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First commit for 9th march 2017
</commit_message>
<xml_diff>
--- a/Neha_Pant.xlsx
+++ b/Neha_Pant.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="243">
   <si>
     <t>S.No</t>
   </si>
@@ -741,6 +741,24 @@
   </si>
   <si>
     <t>Configured billing page with webflow</t>
+  </si>
+  <si>
+    <t>9th Mar,2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Webflow </t>
+  </si>
+  <si>
+    <t>Spring security</t>
+  </si>
+  <si>
+    <t>Cart implementation</t>
+  </si>
+  <si>
+    <t>pending</t>
+  </si>
+  <si>
+    <t>360 minutes</t>
   </si>
 </sst>
 </file>
@@ -1252,10 +1270,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H103"/>
+  <dimension ref="A1:H107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F107" sqref="F107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3898,6 +3916,92 @@
       </c>
       <c r="H103" s="1" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="28.8">
+      <c r="A104" s="1">
+        <v>103</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="28.8">
+      <c r="A105" s="1">
+        <v>104</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="28.8">
+      <c r="A106" s="1">
+        <v>105</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D106" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="28.8">
+      <c r="A107" s="1">
+        <v>106</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First commit for 10th march 2017
</commit_message>
<xml_diff>
--- a/Neha_Pant.xlsx
+++ b/Neha_Pant.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="256">
   <si>
     <t>S.No</t>
   </si>
@@ -752,20 +752,71 @@
     <t>Spring security</t>
   </si>
   <si>
-    <t>Cart implementation</t>
-  </si>
-  <si>
-    <t>pending</t>
-  </si>
-  <si>
     <t>360 minutes</t>
+  </si>
+  <si>
+    <r>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>java.lang.IllegalStateException: Neither BindingResult nor plain target object for bean name 'product' available as request attribute</t>
+    </r>
+  </si>
+  <si>
+    <t>we have to return an object in the requestmapping method of controller : model.addObject("product",new Product()); </t>
+  </si>
+  <si>
+    <t>BindingResult_Error</t>
+  </si>
+  <si>
+    <t>Product Delete using Modal for Admin</t>
+  </si>
+  <si>
+    <t>StaleStaleException_Error</t>
+  </si>
+  <si>
+    <t>Batch update returned unexpected row count from update [0]; actual row count: 0; expected: 1</t>
+  </si>
+  <si>
+    <t>10th Mar,2017</t>
+  </si>
+  <si>
+    <t>ProductDetails Page</t>
+  </si>
+  <si>
+    <t>180 minutes</t>
+  </si>
+  <si>
+    <t>Cart View Page</t>
+  </si>
+  <si>
+    <t>Cart DTO,DAO,DAOImpl</t>
+  </si>
+  <si>
+    <t>CartItem DTO,DAO,DAOImpl</t>
+  </si>
+  <si>
+    <t>Payment Page</t>
+  </si>
+  <si>
+    <t>Payment DTO</t>
+  </si>
+  <si>
+    <t>CartFlow,CartModel,CartHandler</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -811,6 +862,13 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1262,7 +1320,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1270,10 +1328,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H107"/>
+  <dimension ref="A1:H114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F107" sqref="F107"/>
+    <sheetView tabSelected="1" topLeftCell="A104" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3935,7 +3993,7 @@
         <v>19</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G104" s="1" t="s">
         <v>38</v>
@@ -3961,7 +4019,7 @@
         <v>19</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G105" s="1" t="s">
         <v>38</v>
@@ -3989,19 +4047,219 @@
       <c r="F106" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="G106" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="107" spans="1:8" ht="28.8">
       <c r="A107" s="1">
         <v>106</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>240</v>
+        <v>244</v>
+      </c>
+      <c r="D107" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E107" s="20" t="s">
+        <v>19</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>241</v>
+        <v>34</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H107" s="27" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="28.8">
+      <c r="A108" s="1">
+        <v>107</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D108" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E108" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="28.8">
+      <c r="A109" s="1">
+        <v>108</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D109" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E109" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="28.8">
+      <c r="A110" s="1">
+        <v>109</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D110" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E110" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="28.8">
+      <c r="A111" s="1">
+        <v>110</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D111" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E111" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" ht="28.8">
+      <c r="A112" s="1">
+        <v>111</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D112" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E112" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H112" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="28.8">
+      <c r="A113" s="1">
+        <v>112</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D113" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E113" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" ht="28.8">
+      <c r="A114" s="1">
+        <v>113</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D114" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E114" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -4030,8 +4288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="A12" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4240,11 +4498,27 @@
       </c>
       <c r="E14" s="25"/>
     </row>
-    <row r="15" spans="1:5">
-      <c r="C15" s="29"/>
-      <c r="D15" s="25"/>
-    </row>
-    <row r="16" spans="1:5">
+    <row r="15" spans="1:5" ht="26.4">
+      <c r="A15" s="27" t="s">
+        <v>243</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>242</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="28.8">
+      <c r="A16" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>246</v>
+      </c>
       <c r="C16" s="29"/>
     </row>
     <row r="17" spans="3:3">

</xml_diff>

<commit_message>
First commit for 11th march 2017
</commit_message>
<xml_diff>
--- a/Neha_Pant.xlsx
+++ b/Neha_Pant.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="7752"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="7752" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="day 1" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="270">
   <si>
     <t>S.No</t>
   </si>
@@ -810,6 +810,48 @@
   </si>
   <si>
     <t>CartFlow,CartModel,CartHandler</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Use of @OneToMany or @ManyToMany targeting an unmapped class</t>
+  </si>
+  <si>
+    <t>BeanInstantiation_Error</t>
+  </si>
+  <si>
+    <t>Put @Entity inside every model or DTO class</t>
+  </si>
+  <si>
+    <t>http://stackoverflow.com/questions/4956855/hibernate-problem-use-of-onetomany-or-manytomany-targeting-an-unmapped-clas</t>
+  </si>
+  <si>
+    <t>11th Mar,2017</t>
+  </si>
+  <si>
+    <t>NonStaticContext_Error</t>
+  </si>
+  <si>
+    <t>Element cannot be accessed from the not static context in the testcase</t>
+  </si>
+  <si>
+    <t>instance of DAO has to be declared static.</t>
+  </si>
+  <si>
+    <t>StaticImport_Error</t>
+  </si>
+  <si>
+    <t>Detached object is trying to persist</t>
+  </si>
+  <si>
+    <t>use save in place of persist in addToCart method of DAOImpl</t>
+  </si>
+  <si>
+    <t>assertError not recognised</t>
+  </si>
+  <si>
+    <t>imported org.junit.Assert.* with static keyword</t>
+  </si>
+  <si>
+    <t>Detached_Error</t>
   </si>
 </sst>
 </file>
@@ -1328,10 +1370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H114"/>
+  <dimension ref="A1:H115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A108" sqref="A108"/>
+    <sheetView topLeftCell="A105" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C115" sqref="C115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4178,10 +4220,10 @@
         <v>34</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H111" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="H111" s="27" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="112" spans="1:8" ht="28.8">
@@ -4260,6 +4302,14 @@
       </c>
       <c r="H114" s="1" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="28.8">
+      <c r="A115" s="1">
+        <v>114</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -4286,10 +4336,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4514,30 +4564,77 @@
     </row>
     <row r="16" spans="1:5" ht="28.8">
       <c r="A16" s="27" t="s">
+        <v>257</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>258</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="28.8">
+      <c r="A17" s="27" t="s">
         <v>245</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="C16" s="29"/>
-    </row>
-    <row r="17" spans="3:3">
-      <c r="C17" s="29"/>
-    </row>
-    <row r="18" spans="3:3">
-      <c r="C18" s="29"/>
-    </row>
-    <row r="19" spans="3:3">
-      <c r="C19" s="29"/>
+    </row>
+    <row r="18" spans="1:4" ht="28.8">
+      <c r="A18" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>263</v>
+      </c>
+      <c r="D18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="27" t="s">
+        <v>264</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>268</v>
+      </c>
+      <c r="D19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="27" t="s">
+        <v>269</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D20" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="https://gist.github.com/adamjohnson/5682757"/>
     <hyperlink ref="D9" r:id="rId2" tooltip="https://www.youtube.com/watch?v=oPE6UO9yoK4" display="https://www.youtube.com/watch?v=oPE6UO9yoK4"/>
     <hyperlink ref="D11" r:id="rId3"/>
+    <hyperlink ref="D16" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
commit for 13th march 17
</commit_message>
<xml_diff>
--- a/Neha_Pant.xlsx
+++ b/Neha_Pant.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="7752" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="day 1" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="286">
   <si>
     <t>S.No</t>
   </si>
@@ -852,6 +852,54 @@
   </si>
   <si>
     <t>Detached_Error</t>
+  </si>
+  <si>
+    <t>CartItemsTestCase</t>
+  </si>
+  <si>
+    <t>Payment page with spring and validation</t>
+  </si>
+  <si>
+    <t>Payment DAO and DAOImpl</t>
+  </si>
+  <si>
+    <t>CartWebFlow</t>
+  </si>
+  <si>
+    <t>Billing and shipping address page</t>
+  </si>
+  <si>
+    <t>FrontEndCartCOntroller</t>
+  </si>
+  <si>
+    <t>Invoice Page</t>
+  </si>
+  <si>
+    <t>HandlerTypeMismatchException_Error</t>
+  </si>
+  <si>
+    <t>Handler not found</t>
+  </si>
+  <si>
+    <t xml:space="preserve">after authentication,in dispathcer servlet </t>
+  </si>
+  <si>
+    <t>PropertyNotFoundException_error</t>
+  </si>
+  <si>
+    <t>Property not found</t>
+  </si>
+  <si>
+    <t>annotate controller with component</t>
+  </si>
+  <si>
+    <t>Cart Webflow testing</t>
+  </si>
+  <si>
+    <t>PropertyNotFOund_Error,HandlerTytpeMismatchException_Error</t>
+  </si>
+  <si>
+    <t>Detached_Error,StaticImport_Error</t>
   </si>
 </sst>
 </file>
@@ -1370,10 +1418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H115"/>
+  <dimension ref="A1:H122"/>
   <sheetViews>
-    <sheetView topLeftCell="A105" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C115" sqref="C115"/>
+    <sheetView tabSelected="1" topLeftCell="A113" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H115" sqref="H115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4310,6 +4358,206 @@
       </c>
       <c r="B115" s="1" t="s">
         <v>260</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D115" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E115" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H115" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="28.8">
+      <c r="A116" s="1">
+        <v>115</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D116" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E116" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="28.8">
+      <c r="A117" s="1">
+        <v>116</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D117" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E117" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H117" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" ht="28.8">
+      <c r="A118" s="1">
+        <v>117</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D118" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E118" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H118" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="28.8">
+      <c r="A119" s="1">
+        <v>118</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D119" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E119" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H119" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" ht="28.8">
+      <c r="A120" s="1">
+        <v>119</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D120" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E120" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G120" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H120" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="28.8">
+      <c r="A121" s="1">
+        <v>120</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="D121" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E121" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G121" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H121" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="43.2">
+      <c r="A122" s="1">
+        <v>121</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D122" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E122" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G122" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H122" s="1" t="s">
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -4336,10 +4584,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView topLeftCell="A13" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4583,6 +4831,12 @@
       <c r="B17" s="1" t="s">
         <v>246</v>
       </c>
+      <c r="C17" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D17" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="18" spans="1:4" ht="28.8">
       <c r="A18" s="27" t="s">
@@ -4623,6 +4877,34 @@
         <v>266</v>
       </c>
       <c r="D20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="27" t="s">
+        <v>277</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="27" t="s">
+        <v>280</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D22" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>